<commit_message>
Pronósticos hasta 2026 (2000-Q2 a 2027-Q1)
</commit_message>
<xml_diff>
--- a/Quarterly_Yearly_Forecast.xlsx
+++ b/Quarterly_Yearly_Forecast.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unaledu-my.sharepoint.com/personal/msramirezgo_unal_edu_co/Documents/Oliver Pardo/VAR_VEC-2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="522" documentId="13_ncr:1_{E745283E-EFC1-4155-822F-BC1E14BD8D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD057A5D-0D2C-4C49-B197-834AE2661815}"/>
+  <xr:revisionPtr revIDLastSave="572" documentId="13_ncr:1_{E745283E-EFC1-4155-822F-BC1E14BD8D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84831B2A-6127-4E17-A632-FB4F83CD829E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue Current" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="122">
   <si>
     <t>Lower CI</t>
   </si>
@@ -396,6 +396,18 @@
   <si>
     <t>2026-Q1</t>
   </si>
+  <si>
+    <t>2026-Q2</t>
+  </si>
+  <si>
+    <t>2026-Q3</t>
+  </si>
+  <si>
+    <t>2026-Q4</t>
+  </si>
+  <si>
+    <t>2027-Q1</t>
+  </si>
 </sst>
 </file>
 
@@ -12832,10 +12844,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Revenue Current Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Revenue Current Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -12913,16 +12925,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Revenue Current Yearly'!$B$2:$B$27</c:f>
+              <c:f>'Revenue Current Yearly'!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>338.78899999999999</c:v>
                 </c:pt>
@@ -13000,6 +13015,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1442.2107850635657</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1525.5594289730946</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13049,10 +13067,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Revenue Current Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Revenue Current Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -13130,16 +13148,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Revenue Current Yearly'!$C$2:$C$27</c:f>
+              <c:f>'Revenue Current Yearly'!$C$2:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -13217,6 +13238,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1306.1883870575348</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1386.7753065575944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13266,10 +13290,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Revenue Current Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Revenue Current Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -13347,16 +13371,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Revenue Current Yearly'!$D$2:$D$27</c:f>
+              <c:f>'Revenue Current Yearly'!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -13434,6 +13461,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1578.2331830695966</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1664.3435513885947</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13502,13 +13532,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Revenue Current Yearly'!$A$2:$A$27</c15:sqref>
+                          <c15:sqref>'Revenue Current Yearly'!$A$2:$A$28</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="27"/>
                       <c:pt idx="0">
                         <c:v>2000</c:v>
                       </c:pt>
@@ -13586,6 +13616,9 @@
                       </c:pt>
                       <c:pt idx="25">
                         <c:v>2025</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2026</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -14000,10 +14033,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Total Revenue and Grants Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Total Revenue and Grants Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -14081,16 +14114,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Revenue and Grants Yearly'!$B$2:$B$27</c:f>
+              <c:f>'Total Revenue and Grants Yearly'!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>434.26800000000003</c:v>
                 </c:pt>
@@ -14168,6 +14204,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1444.6057119050956</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1519.5985902004227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14217,10 +14256,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Total Revenue and Grants Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Total Revenue and Grants Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -14298,16 +14337,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Revenue and Grants Yearly'!$C$2:$C$27</c:f>
+              <c:f>'Total Revenue and Grants Yearly'!$C$2:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -14385,6 +14427,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1313.8538618440098</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1386.6150930915358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14434,10 +14479,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Total Revenue and Grants Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Total Revenue and Grants Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -14515,16 +14560,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Total Revenue and Grants Yearly'!$D$2:$D$27</c:f>
+              <c:f>'Total Revenue and Grants Yearly'!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -14602,6 +14650,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1575.3575619661815</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1652.5820873093096</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14670,13 +14721,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Total Revenue and Grants Yearly'!$A$2:$A$27</c15:sqref>
+                          <c15:sqref>'Total Revenue and Grants Yearly'!$A$2:$A$28</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="27"/>
                       <c:pt idx="0">
                         <c:v>2000</c:v>
                       </c:pt>
@@ -14754,6 +14805,9 @@
                       </c:pt>
                       <c:pt idx="25">
                         <c:v>2025</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2026</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -15168,10 +15222,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Expenditure Current Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Expenditure Current Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -15249,16 +15303,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Expenditure Current Yearly'!$B$2:$B$27</c:f>
+              <c:f>'Expenditure Current Yearly'!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>295.76200000000006</c:v>
                 </c:pt>
@@ -15336,6 +15393,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1095.0039782797107</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1150.3546858480504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15385,10 +15445,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Expenditure Current Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Expenditure Current Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -15466,16 +15526,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Expenditure Current Yearly'!$C$2:$C$27</c:f>
+              <c:f>'Expenditure Current Yearly'!$C$2:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -15553,6 +15616,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>990.78630790072702</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1050.6111787312725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15602,10 +15668,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Expenditure Current Yearly'!$A$2:$A$27</c:f>
+              <c:f>'Expenditure Current Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -15683,16 +15749,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Expenditure Current Yearly'!$D$2:$D$27</c:f>
+              <c:f>'Expenditure Current Yearly'!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -15770,6 +15839,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1199.2216486586944</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1250.0981929648283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15838,13 +15910,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Expenditure Current Yearly'!$A$2:$A$27</c15:sqref>
+                          <c15:sqref>'Expenditure Current Yearly'!$A$2:$A$28</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="27"/>
                       <c:pt idx="0">
                         <c:v>2000</c:v>
                       </c:pt>
@@ -15922,6 +15994,9 @@
                       </c:pt>
                       <c:pt idx="25">
                         <c:v>2025</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2026</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -16336,10 +16411,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>' Total Expenditure Yearly'!$A$2:$A$27</c:f>
+              <c:f>' Total Expenditure Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -16417,16 +16492,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>' Total Expenditure Yearly'!$B$2:$B$27</c:f>
+              <c:f>' Total Expenditure Yearly'!$B$2:$B$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>527.18600000000015</c:v>
                 </c:pt>
@@ -16504,6 +16582,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1371.3125124074327</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1427.8801718321931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16553,10 +16634,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>' Total Expenditure Yearly'!$A$2:$A$27</c:f>
+              <c:f>' Total Expenditure Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -16634,16 +16715,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>' Total Expenditure Yearly'!$C$2:$C$27</c:f>
+              <c:f>' Total Expenditure Yearly'!$C$2:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -16721,6 +16805,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1242.0068873429266</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1298.7745191479753</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16770,10 +16857,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>' Total Expenditure Yearly'!$A$2:$A$27</c:f>
+              <c:f>' Total Expenditure Yearly'!$A$2:$A$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -16851,16 +16938,19 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>' Total Expenditure Yearly'!$D$2:$D$27</c:f>
+              <c:f>' Total Expenditure Yearly'!$D$2:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="26"/>
+                <c:ptCount val="27"/>
                 <c:pt idx="0">
                   <c:v>#N/A</c:v>
                 </c:pt>
@@ -16938,6 +17028,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1500.6181374719388</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1556.985824516411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17006,13 +17099,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>' Total Expenditure Yearly'!$A$2:$A$27</c15:sqref>
+                          <c15:sqref>' Total Expenditure Yearly'!$A$2:$A$28</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="26"/>
+                      <c:ptCount val="27"/>
                       <c:pt idx="0">
                         <c:v>2000</c:v>
                       </c:pt>
@@ -17090,6 +17183,9 @@
                       </c:pt>
                       <c:pt idx="25">
                         <c:v>2025</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>2026</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -22064,6 +22160,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -22361,10 +22461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9AB4B5-1BE8-4F17-BBE0-77B710584B11}">
-  <dimension ref="A1:R106"/>
+  <dimension ref="A1:R110"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105:E106"/>
+    <sheetView topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24226,6 +24326,82 @@
         <v>401.99808305372181</v>
       </c>
     </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="9">
+        <v>373.2889353942943</v>
+      </c>
+      <c r="C107" s="9">
+        <v>1481.9386609142243</v>
+      </c>
+      <c r="D107" s="10">
+        <f t="shared" ref="D107:D110" si="4">B107-(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>338.5442491327421</v>
+      </c>
+      <c r="E107" s="10">
+        <f t="shared" ref="E107:E110" si="5">B107+(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>408.0336216558465</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="9">
+        <v>379.06743235760428</v>
+      </c>
+      <c r="C108" s="9">
+        <v>1492.2675844856878</v>
+      </c>
+      <c r="D108" s="10">
+        <f t="shared" si="4"/>
+        <v>344.1824256510431</v>
+      </c>
+      <c r="E108" s="10">
+        <f t="shared" si="5"/>
+        <v>413.95243906416545</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="9">
+        <v>384.04818318039662</v>
+      </c>
+      <c r="C109" s="9">
+        <v>1500.8828624354255</v>
+      </c>
+      <c r="D109" s="10">
+        <f t="shared" si="4"/>
+        <v>348.8438325971548</v>
+      </c>
+      <c r="E109" s="10">
+        <f t="shared" si="5"/>
+        <v>419.25253376363844</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="9">
+        <v>389.15487804079925</v>
+      </c>
+      <c r="C110" s="9">
+        <v>1516.4609719854836</v>
+      </c>
+      <c r="D110" s="10">
+        <f t="shared" si="4"/>
+        <v>353.75822450444451</v>
+      </c>
+      <c r="E110" s="10">
+        <f t="shared" si="5"/>
+        <v>424.55153157715398</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24236,10 +24412,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4A1349-5152-4296-BA6A-B5CBC0E8B26F}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+      <selection activeCell="D106" sqref="D106:E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26090,6 +26266,82 @@
         <v>402.42344909571136</v>
       </c>
     </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="9">
+        <v>373.02472386089346</v>
+      </c>
+      <c r="C107" s="9">
+        <v>1652.7055891132879</v>
+      </c>
+      <c r="D107" s="10">
+        <f t="shared" ref="D107:D110" si="4">B107-(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>339.46437578666593</v>
+      </c>
+      <c r="E107" s="10">
+        <f t="shared" ref="E107:E110" si="5">B107+(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>406.58507193512099</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="9">
+        <v>376.75800311702432</v>
+      </c>
+      <c r="C108" s="9">
+        <v>1664.5465471150876</v>
+      </c>
+      <c r="D108" s="10">
+        <f t="shared" si="4"/>
+        <v>343.1080487968141</v>
+      </c>
+      <c r="E108" s="10">
+        <f t="shared" si="5"/>
+        <v>410.40795743723453</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="9">
+        <v>382.09699837132547</v>
+      </c>
+      <c r="C109" s="9">
+        <v>1688.3756467184492</v>
+      </c>
+      <c r="D109" s="10">
+        <f t="shared" si="4"/>
+        <v>348.04329996579395</v>
+      </c>
+      <c r="E109" s="10">
+        <f t="shared" si="5"/>
+        <v>416.15069677685699</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="9">
+        <v>387.71886485117943</v>
+      </c>
+      <c r="C110" s="9">
+        <v>1710.7771996741903</v>
+      </c>
+      <c r="D110" s="10">
+        <f t="shared" si="4"/>
+        <v>353.64341953045795</v>
+      </c>
+      <c r="E110" s="10">
+        <f t="shared" si="5"/>
+        <v>421.79431017190092</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -26099,10 +26351,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD733903-6132-4601-82D1-0EC76750991E}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105:E106"/>
+      <selection activeCell="D106" sqref="D106:E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27953,6 +28205,82 @@
         <v>306.92830635937855</v>
       </c>
     </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="9">
+        <v>280.55740965453174</v>
+      </c>
+      <c r="C107" s="9">
+        <v>1421.2982517139858</v>
+      </c>
+      <c r="D107" s="10">
+        <f t="shared" ref="D107:D110" si="4">B107-(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>255.00411074740487</v>
+      </c>
+      <c r="E107" s="10">
+        <f t="shared" ref="E107:E110" si="5">B107+(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>306.11070856165861</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="9">
+        <v>287.48954034826403</v>
+      </c>
+      <c r="C108" s="9">
+        <v>1432.3828977911344</v>
+      </c>
+      <c r="D108" s="10">
+        <f t="shared" si="4"/>
+        <v>262.24290450548932</v>
+      </c>
+      <c r="E108" s="10">
+        <f t="shared" si="5"/>
+        <v>312.73617619103874</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="9">
+        <v>288.13190139134912</v>
+      </c>
+      <c r="C109" s="9">
+        <v>1448.8076125072487</v>
+      </c>
+      <c r="D109" s="10">
+        <f t="shared" si="4"/>
+        <v>263.06244462070958</v>
+      </c>
+      <c r="E109" s="10">
+        <f t="shared" si="5"/>
+        <v>313.20135816198865</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="9">
+        <v>294.17583445390557</v>
+      </c>
+      <c r="C110" s="9">
+        <v>1457.6731990875276</v>
+      </c>
+      <c r="D110" s="10">
+        <f t="shared" si="4"/>
+        <v>269.27871449687427</v>
+      </c>
+      <c r="E110" s="10">
+        <f t="shared" si="5"/>
+        <v>319.07295441093686</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -27962,10 +28290,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+      <selection activeCell="D106" sqref="D106:E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29816,6 +30144,82 @@
         <v>382.62662726630799</v>
       </c>
     </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="9">
+        <v>349.6780335101663</v>
+      </c>
+      <c r="C107" s="9">
+        <v>1633.4056220746966</v>
+      </c>
+      <c r="D107" s="10">
+        <f t="shared" ref="D107:D110" si="4">B107-(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>316.29040151925352</v>
+      </c>
+      <c r="E107" s="10">
+        <f t="shared" ref="E107:E110" si="5">B107+(_xlfn.STDEV.P(B17:B106)/2)</f>
+        <v>383.06566550107908</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B108" s="9">
+        <v>354.81982678266712</v>
+      </c>
+      <c r="C108" s="9">
+        <v>1646.0704352157993</v>
+      </c>
+      <c r="D108" s="10">
+        <f t="shared" si="4"/>
+        <v>321.56806183264945</v>
+      </c>
+      <c r="E108" s="10">
+        <f t="shared" si="5"/>
+        <v>388.07159173268479</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B109" s="9">
+        <v>360.60212244825976</v>
+      </c>
+      <c r="C109" s="9">
+        <v>1683.6013836236648</v>
+      </c>
+      <c r="D109" s="10">
+        <f t="shared" si="4"/>
+        <v>327.2287494487756</v>
+      </c>
+      <c r="E109" s="10">
+        <f t="shared" si="5"/>
+        <v>393.97549544774392</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B110" s="9">
+        <v>362.7801890911</v>
+      </c>
+      <c r="C110" s="9">
+        <v>1703.842078091885</v>
+      </c>
+      <c r="D110" s="10">
+        <f t="shared" si="4"/>
+        <v>329.51571057318603</v>
+      </c>
+      <c r="E110" s="10">
+        <f t="shared" si="5"/>
+        <v>396.04466760901397</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -29826,10 +30230,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62DE25F-4940-44D7-8659-54912D442C92}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30403,6 +30807,27 @@
         <v>1371.3125124074327</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B28" s="10">
+        <f>SUM('Revenue Current'!$B$107:$B$110)</f>
+        <v>1525.5594289730946</v>
+      </c>
+      <c r="C28" s="10">
+        <f>SUM('Total Revenue and Grants'!$B$107:$B$110)</f>
+        <v>1519.5985902004227</v>
+      </c>
+      <c r="D28" s="10">
+        <f>SUM( 'Expenditure Current'!$B$107:$B$110)</f>
+        <v>1150.3546858480504</v>
+      </c>
+      <c r="E28" s="10">
+        <f>SUM( 'Total Expenditure'!$B$107:$B$110)</f>
+        <v>1427.8801718321931</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30410,10 +30835,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470B3BD9-D9D9-411A-BFE7-DE787F2A6341}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B27"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30442,7 +30867,6 @@
         <v>2000</v>
       </c>
       <c r="B2" s="15">
-        <f>SUM('Revenue Current'!$B$3:$B$6)</f>
         <v>338.78899999999999</v>
       </c>
       <c r="C2" s="15" t="e">
@@ -30457,7 +30881,6 @@
         <v>2001</v>
       </c>
       <c r="B3" s="15">
-        <f>SUM('Revenue Current'!$B$7:$B$10)</f>
         <v>402.37299999999999</v>
       </c>
       <c r="C3" s="15" t="e">
@@ -30472,7 +30895,6 @@
         <v>2002</v>
       </c>
       <c r="B4" s="15">
-        <f>SUM('Revenue Current'!$B$11:$B$14)</f>
         <v>411.66599999999994</v>
       </c>
       <c r="C4" s="15" t="e">
@@ -30487,7 +30909,6 @@
         <v>2003</v>
       </c>
       <c r="B5" s="15">
-        <f>SUM('Revenue Current'!$B$15:$B$18)</f>
         <v>433.37099999999998</v>
       </c>
       <c r="C5" s="15" t="e">
@@ -30502,7 +30923,6 @@
         <v>2004</v>
       </c>
       <c r="B6" s="15">
-        <f>SUM('Revenue Current'!$B$19:$B$22)</f>
         <v>456.22800000000007</v>
       </c>
       <c r="C6" s="15" t="e">
@@ -30517,7 +30937,6 @@
         <v>2005</v>
       </c>
       <c r="B7" s="15">
-        <f>SUM('Revenue Current'!$B$23:$B$26)</f>
         <v>529.82000000000005</v>
       </c>
       <c r="C7" s="15" t="e">
@@ -30532,7 +30951,6 @@
         <v>2006</v>
       </c>
       <c r="B8" s="15">
-        <f>SUM('Revenue Current'!$B$27:$B$30)</f>
         <v>586.46500000000003</v>
       </c>
       <c r="C8" s="15" t="e">
@@ -30547,7 +30965,6 @@
         <v>2007</v>
       </c>
       <c r="B9" s="15">
-        <f>SUM('Revenue Current'!$B$31:$B$33)</f>
         <v>495.04500000000007</v>
       </c>
       <c r="C9" s="15" t="e">
@@ -30562,7 +30979,6 @@
         <v>2008</v>
       </c>
       <c r="B10" s="15">
-        <f>SUM('Revenue Current'!$B$34:$B$37)</f>
         <v>732.34400000000005</v>
       </c>
       <c r="C10" s="15" t="e">
@@ -30577,7 +30993,6 @@
         <v>2009</v>
       </c>
       <c r="B11" s="15">
-        <f>SUM('Revenue Current'!$B$39:$B$42)</f>
         <v>696.73216238000009</v>
       </c>
       <c r="C11" s="15" t="e">
@@ -30592,7 +31007,6 @@
         <v>2010</v>
       </c>
       <c r="B12" s="15">
-        <f>SUM('Revenue Current'!$B$43:$B$46)</f>
         <v>766.15637277488065</v>
       </c>
       <c r="C12" s="15" t="e">
@@ -30607,7 +31021,6 @@
         <v>2011</v>
       </c>
       <c r="B13" s="15">
-        <f>SUM('Revenue Current'!$B$47:$B$50)</f>
         <v>795.86856776000013</v>
       </c>
       <c r="C13" s="15" t="e">
@@ -30622,7 +31035,6 @@
         <v>2012</v>
       </c>
       <c r="B14" s="15">
-        <f>SUM('Revenue Current'!$B$51:$B$54)</f>
         <v>814.36172873000021</v>
       </c>
       <c r="C14" s="15" t="e">
@@ -30637,7 +31049,6 @@
         <v>2013</v>
       </c>
       <c r="B15" s="15">
-        <f>SUM('Revenue Current'!$B$55:$B$58)</f>
         <v>865.90432022999994</v>
       </c>
       <c r="C15" s="15" t="e">
@@ -30652,7 +31063,6 @@
         <v>2014</v>
       </c>
       <c r="B16" s="15">
-        <f>SUM('Revenue Current'!$B$59:$B$62)</f>
         <v>960.80008016099998</v>
       </c>
       <c r="C16" s="15" t="e">
@@ -30667,7 +31077,6 @@
         <v>2015</v>
       </c>
       <c r="B17" s="15">
-        <f>SUM('Revenue Current'!$B$63:$B$66)</f>
         <v>972.88620311</v>
       </c>
       <c r="C17" s="15" t="e">
@@ -30682,7 +31091,6 @@
         <v>2016</v>
       </c>
       <c r="B18" s="15">
-        <f>SUM('Revenue Current'!$B$67:$B$70)</f>
         <v>1004.0287535799998</v>
       </c>
       <c r="C18" s="15" t="e">
@@ -30697,7 +31105,6 @@
         <v>2017</v>
       </c>
       <c r="B19" s="15">
-        <f>SUM('Revenue Current'!$B$71:$B$74)</f>
         <v>1087.9859353200002</v>
       </c>
       <c r="C19" s="15" t="e">
@@ -30712,7 +31119,6 @@
         <v>2018</v>
       </c>
       <c r="B20" s="15">
-        <f>SUM('Revenue Current'!$B$75:$B$78)</f>
         <v>1144.1160055400001</v>
       </c>
       <c r="C20" s="15" t="e">
@@ -30727,7 +31133,6 @@
         <v>2019</v>
       </c>
       <c r="B21" s="15">
-        <f>SUM('Revenue Current'!$B$79:$B$82)</f>
         <v>1141.9491431699998</v>
       </c>
       <c r="C21" s="15" t="e">
@@ -30742,7 +31147,6 @@
         <v>2020</v>
       </c>
       <c r="B22" s="15">
-        <f>SUM('Revenue Current'!$B$83:$B$86)</f>
         <v>874.59354385999995</v>
       </c>
       <c r="C22" s="15" t="e">
@@ -30757,7 +31161,6 @@
         <v>2021</v>
       </c>
       <c r="B23" s="15">
-        <f>SUM('Revenue Current'!$B$87:$B$90)</f>
         <v>1164.9753499599999</v>
       </c>
       <c r="C23" s="15">
@@ -30774,7 +31177,6 @@
         <v>2022</v>
       </c>
       <c r="B24" s="10">
-        <f>SUM('Revenue Current'!$B$91:$B$94)</f>
         <v>1220.0970610729307</v>
       </c>
       <c r="C24" s="10">
@@ -30791,7 +31193,6 @@
         <v>2023</v>
       </c>
       <c r="B25" s="10">
-        <f>SUM('Revenue Current'!$B$95:$B$98)</f>
         <v>1291.0773702930728</v>
       </c>
       <c r="C25" s="10">
@@ -30808,7 +31209,6 @@
         <v>2024</v>
       </c>
       <c r="B26" s="10">
-        <f>SUM('Revenue Current'!$B$99:$B$102)</f>
         <v>1363.957623438894</v>
       </c>
       <c r="C26" s="10">
@@ -30825,7 +31225,6 @@
         <v>2025</v>
       </c>
       <c r="B27" s="10">
-        <f>SUM('Revenue Current'!$B$103:$B$106)</f>
         <v>1442.2107850635657</v>
       </c>
       <c r="C27" s="10">
@@ -30835,6 +31234,22 @@
       <c r="D27" s="10">
         <f t="shared" si="1"/>
         <v>1578.2331830695966</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1525.5594289730946</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" ref="C28" si="2">B28-_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1386.7753065575944</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" ref="D28" si="3">B28+_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1664.3435513885947</v>
       </c>
     </row>
   </sheetData>
@@ -30846,10 +31261,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFCA7D2A-0085-44C6-974D-1E6E00F6E585}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31273,6 +31688,23 @@
         <v>1575.3575619661815</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B28" s="10">
+        <f>SUM('Total Revenue and Grants'!$B$107:$B$110)</f>
+        <v>1519.5985902004227</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" ref="C28" si="2">B28-_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1386.6150930915358</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" ref="D28" si="3">B28+_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1652.5820873093096</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31282,10 +31714,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1E5342-B4E2-43A6-AE60-EDF98511EA1F}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31709,6 +32141,23 @@
         <v>1199.2216486586944</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B28" s="10">
+        <f>SUM( 'Expenditure Current'!$B$107:$B$110)</f>
+        <v>1150.3546858480504</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" ref="C28" si="2">B28-_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1050.6111787312725</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" ref="D28" si="3">B28+_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1250.0981929648283</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31718,10 +32167,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BFFC21-10E3-4D87-95C6-8106DC0C8D0D}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32145,6 +32594,23 @@
         <v>1500.6181374719388</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2026</v>
+      </c>
+      <c r="B28" s="10">
+        <f>SUM( 'Total Expenditure'!$B$107:$B$110)</f>
+        <v>1427.8801718321931</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" ref="C28" si="2">B28-_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1298.7745191479753</v>
+      </c>
+      <c r="D28" s="10">
+        <f t="shared" ref="D28" si="3">B28+_xlfn.STDEV.P(B6:B27)/2</f>
+        <v>1556.985824516411</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>